<commit_message>
We found out that the three journals we thought stop accepting submissions simply have changed publishers. We updated the information about the code-policy in the database.
</commit_message>
<xml_diff>
--- a/data/Updated_Table_Mislan_2020_v2.xlsx
+++ b/data/Updated_Table_Mislan_2020_v2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="268">
   <si>
     <t>Full Journal Title</t>
   </si>
@@ -452,15 +452,9 @@
     <t>http://onlinelibrary.wiley.com/journal/10.1111/(ISSN)1442-9993</t>
   </si>
   <si>
-    <t>http://link.springer.com/journal/10144</t>
-  </si>
-  <si>
     <t>Norwegian Polar Institute</t>
   </si>
   <si>
-    <t>http://onlinelibrary.wiley.com/journal/10.1111/(ISSN)1751-8369</t>
-  </si>
-  <si>
     <t>http://www.journals.elsevier.com/pedobiologia/</t>
   </si>
   <si>
@@ -482,9 +476,6 @@
     <t>Ecological Society of Japan</t>
   </si>
   <si>
-    <t>http://link.springer.com/journal/11284</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rangeland Ecology &amp; Management </t>
   </si>
   <si>
@@ -797,9 +788,6 @@
     <t>Mandatory</t>
   </si>
   <si>
-    <t>Journal no longer exist</t>
-  </si>
-  <si>
     <t>Comment_on_2020</t>
   </si>
   <si>
@@ -824,9 +812,6 @@
     <t xml:space="preserve">They do not mention code, but at the same time say: "All data sources, models, and other information must be fully documented." </t>
   </si>
   <si>
-    <t>Last issue 2018</t>
-  </si>
-  <si>
     <t xml:space="preserve">Though at least they mention the following: "Note: if data, scripts, or other artefacts used to generate the analyses presented in the paper are available via a publicly available data repository, authors should include a reference to the location of the material within their paper." </t>
   </si>
   <si>
@@ -834,6 +819,18 @@
   </si>
   <si>
     <t>Require computer code with publication_2020</t>
+  </si>
+  <si>
+    <t>Journal changed publisher</t>
+  </si>
+  <si>
+    <t>https://esj-journals.onlinelibrary.wiley.com/journal/14401703</t>
+  </si>
+  <si>
+    <t>https://besjournals.onlinelibrary.wiley.com/hub/PolarEcology2018</t>
+  </si>
+  <si>
+    <t>https://polarresearch.net/index.php/polar/about</t>
   </si>
 </sst>
 </file>
@@ -910,13 +907,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="5" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -1264,7 +1262,7 @@
   <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F86" sqref="F86"/>
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1289,21 +1287,21 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -1321,7 +1319,7 @@
     </row>
     <row r="3" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
@@ -1336,7 +1334,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G3" s="3"/>
     </row>
@@ -1345,7 +1343,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>12</v>
@@ -1378,13 +1376,13 @@
         <v>6</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>18</v>
@@ -1405,10 +1403,10 @@
     </row>
     <row r="7" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -1423,15 +1421,15 @@
         <v>6</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
@@ -1443,13 +1441,13 @@
         <v>6</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
@@ -1464,16 +1462,16 @@
         <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>8</v>
@@ -1485,13 +1483,13 @@
         <v>10</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>24</v>
@@ -1506,7 +1504,7 @@
         <v>10</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G11" s="3"/>
     </row>
@@ -1515,7 +1513,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
@@ -1527,16 +1525,16 @@
         <v>10</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>8</v>
@@ -1548,7 +1546,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G13" s="3"/>
     </row>
@@ -1569,13 +1567,13 @@
         <v>10</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>31</v>
@@ -1590,13 +1588,13 @@
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>18</v>
@@ -1611,16 +1609,16 @@
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>8</v>
@@ -1632,13 +1630,13 @@
         <v>6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>24</v>
@@ -1653,13 +1651,13 @@
         <v>10</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>24</v>
@@ -1674,13 +1672,13 @@
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
@@ -1695,13 +1693,13 @@
         <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>39</v>
@@ -1716,13 +1714,13 @@
         <v>6</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>41</v>
@@ -1737,13 +1735,13 @@
         <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>44</v>
@@ -1758,13 +1756,13 @@
         <v>6</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>46</v>
@@ -1779,13 +1777,13 @@
         <v>6</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>48</v>
@@ -1800,13 +1798,13 @@
         <v>10</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>50</v>
@@ -1821,13 +1819,13 @@
         <v>6</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>53</v>
@@ -1842,7 +1840,7 @@
         <v>10</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G27" s="3"/>
     </row>
@@ -1863,16 +1861,16 @@
         <v>6</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>59</v>
@@ -1890,7 +1888,7 @@
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>46</v>
@@ -1911,10 +1909,10 @@
     </row>
     <row r="31" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>59</v>
@@ -1932,7 +1930,7 @@
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>63</v>
@@ -1947,7 +1945,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G32" s="3"/>
     </row>
@@ -1968,13 +1966,13 @@
         <v>6</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>67</v>
@@ -1989,16 +1987,16 @@
         <v>6</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>51</v>
@@ -2010,16 +2008,16 @@
         <v>6</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>59</v>
@@ -2037,10 +2035,10 @@
     </row>
     <row r="37" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>51</v>
@@ -2052,13 +2050,13 @@
         <v>6</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>72</v>
@@ -2079,10 +2077,10 @@
     </row>
     <row r="39" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>59</v>
@@ -2097,15 +2095,15 @@
         <v>6</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>59</v>
@@ -2120,15 +2118,15 @@
         <v>6</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>51</v>
@@ -2140,13 +2138,13 @@
         <v>6</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G41" s="3"/>
     </row>
     <row r="42" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>78</v>
@@ -2161,13 +2159,13 @@
         <v>6</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G42" s="3"/>
     </row>
     <row r="43" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>80</v>
@@ -2182,16 +2180,16 @@
         <v>6</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G43" s="3"/>
     </row>
     <row r="44" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>59</v>
@@ -2203,16 +2201,16 @@
         <v>6</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G44" s="3"/>
     </row>
     <row r="45" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>83</v>
@@ -2230,10 +2228,10 @@
     </row>
     <row r="46" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>85</v>
@@ -2245,16 +2243,16 @@
         <v>6</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G46" s="3"/>
     </row>
     <row r="47" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>87</v>
@@ -2269,7 +2267,7 @@
         <v>6</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
@@ -2277,7 +2275,7 @@
         <v>89</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>8</v>
@@ -2289,16 +2287,16 @@
         <v>6</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G48" s="3"/>
     </row>
     <row r="49" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>51</v>
@@ -2310,7 +2308,7 @@
         <v>6</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G49" s="3"/>
     </row>
@@ -2331,13 +2329,13 @@
         <v>10</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G50" s="3"/>
     </row>
     <row r="51" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>94</v>
@@ -2352,13 +2350,13 @@
         <v>6</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G51" s="3"/>
     </row>
     <row r="52" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>96</v>
@@ -2373,16 +2371,16 @@
         <v>6</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G52" s="3"/>
     </row>
     <row r="53" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>59</v>
@@ -2394,16 +2392,16 @@
         <v>6</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G53" s="3"/>
     </row>
     <row r="54" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>51</v>
@@ -2415,13 +2413,13 @@
         <v>6</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G54" s="3"/>
     </row>
     <row r="55" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>100</v>
@@ -2439,12 +2437,12 @@
         <v>6</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>67</v>
@@ -2459,13 +2457,13 @@
         <v>6</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G56" s="3"/>
     </row>
     <row r="57" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>104</v>
@@ -2486,10 +2484,10 @@
     </row>
     <row r="58" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>59</v>
@@ -2501,13 +2499,13 @@
         <v>6</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G58" s="3"/>
     </row>
     <row r="59" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>107</v>
@@ -2522,7 +2520,7 @@
         <v>6</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G59" s="3"/>
     </row>
@@ -2549,10 +2547,10 @@
     </row>
     <row r="61" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>51</v>
@@ -2564,13 +2562,13 @@
         <v>6</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>113</v>
@@ -2585,16 +2583,16 @@
         <v>6</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>59</v>
@@ -2606,16 +2604,16 @@
         <v>6</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>59</v>
@@ -2627,7 +2625,7 @@
         <v>6</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G64" s="3"/>
     </row>
@@ -2636,7 +2634,7 @@
         <v>117</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>51</v>
@@ -2648,13 +2646,13 @@
         <v>6</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>119</v>
@@ -2669,7 +2667,7 @@
         <v>6</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G66" s="3"/>
     </row>
@@ -2678,7 +2676,7 @@
         <v>121</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>51</v>
@@ -2690,16 +2688,16 @@
         <v>6</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G67" s="3"/>
     </row>
     <row r="68" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>59</v>
@@ -2711,13 +2709,13 @@
         <v>6</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>124</v>
@@ -2735,15 +2733,15 @@
         <v>6</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>87</v>
@@ -2758,15 +2756,15 @@
         <v>6</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>51</v>
@@ -2778,13 +2776,13 @@
         <v>6</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>128</v>
@@ -2799,16 +2797,16 @@
         <v>6</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>51</v>
@@ -2820,13 +2818,13 @@
         <v>6</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>131</v>
@@ -2844,15 +2842,15 @@
         <v>6</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>134</v>
@@ -2870,10 +2868,10 @@
     </row>
     <row r="76" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>59</v>
@@ -2885,7 +2883,7 @@
         <v>6</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G76" s="3"/>
     </row>
@@ -2894,7 +2892,7 @@
         <v>137</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>59</v>
@@ -2906,13 +2904,13 @@
         <v>6</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G77" s="3"/>
     </row>
     <row r="78" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>139</v>
@@ -2927,85 +2925,89 @@
         <v>6</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G78" s="3"/>
     </row>
     <row r="79" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D79" s="2" t="s">
-        <v>141</v>
+      <c r="D79" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="E79" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F79" s="1"/>
+      <c r="F79" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="G79" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D80" s="2" t="s">
-        <v>143</v>
+      <c r="D80" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="E80" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F80" s="1"/>
+      <c r="F80" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="G80" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E81" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G81" s="3"/>
     </row>
     <row r="82" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E82" s="1" t="s">
         <v>6</v>
@@ -3014,33 +3016,33 @@
         <v>6</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E83" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G83" s="3"/>
     </row>
     <row r="84" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>80</v>
@@ -3049,154 +3051,156 @@
         <v>8</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G84" s="3"/>
     </row>
     <row r="85" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E85" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G85" s="3"/>
     </row>
     <row r="86" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D86" s="2" t="s">
-        <v>151</v>
+      <c r="D86" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="E86" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F86" s="1"/>
+      <c r="F86" s="1" t="s">
+        <v>249</v>
+      </c>
       <c r="G86" s="1" t="s">
-        <v>256</v>
+        <v>264</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="E87" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G87" s="3"/>
     </row>
     <row r="88" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E88" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G88" s="3"/>
     </row>
     <row r="89" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G89" s="3"/>
     </row>
     <row r="90" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G90" s="3"/>
     </row>
     <row r="91" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>6</v>
@@ -3208,121 +3212,121 @@
     </row>
     <row r="92" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G92" s="3"/>
     </row>
     <row r="93" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G93" s="3"/>
     </row>
     <row r="94" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E94" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G94" s="3"/>
     </row>
     <row r="95" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G95" s="3"/>
     </row>
     <row r="96" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="G96" s="3"/>
     </row>
     <row r="97" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>6</v>
@@ -3413,24 +3417,24 @@
     <hyperlink ref="D77" r:id="rId76"/>
     <hyperlink ref="D78" r:id="rId77"/>
     <hyperlink ref="D79" r:id="rId78"/>
-    <hyperlink ref="D80" r:id="rId79"/>
-    <hyperlink ref="D81" r:id="rId80"/>
-    <hyperlink ref="D82" r:id="rId81"/>
-    <hyperlink ref="D83" r:id="rId82"/>
-    <hyperlink ref="D84" r:id="rId83"/>
-    <hyperlink ref="D85" r:id="rId84"/>
-    <hyperlink ref="D86" r:id="rId85"/>
-    <hyperlink ref="D88" r:id="rId86"/>
-    <hyperlink ref="D89" r:id="rId87"/>
-    <hyperlink ref="D90" r:id="rId88"/>
-    <hyperlink ref="D91" r:id="rId89"/>
-    <hyperlink ref="D92" r:id="rId90"/>
-    <hyperlink ref="D93" r:id="rId91"/>
-    <hyperlink ref="D94" r:id="rId92"/>
-    <hyperlink ref="D95" r:id="rId93"/>
-    <hyperlink ref="D96" r:id="rId94"/>
-    <hyperlink ref="D97" r:id="rId95"/>
-    <hyperlink ref="D87" r:id="rId96"/>
+    <hyperlink ref="D81" r:id="rId79"/>
+    <hyperlink ref="D82" r:id="rId80"/>
+    <hyperlink ref="D83" r:id="rId81"/>
+    <hyperlink ref="D84" r:id="rId82"/>
+    <hyperlink ref="D85" r:id="rId83"/>
+    <hyperlink ref="D86" r:id="rId84"/>
+    <hyperlink ref="D88" r:id="rId85"/>
+    <hyperlink ref="D89" r:id="rId86"/>
+    <hyperlink ref="D90" r:id="rId87"/>
+    <hyperlink ref="D91" r:id="rId88"/>
+    <hyperlink ref="D92" r:id="rId89"/>
+    <hyperlink ref="D93" r:id="rId90"/>
+    <hyperlink ref="D94" r:id="rId91"/>
+    <hyperlink ref="D95" r:id="rId92"/>
+    <hyperlink ref="D96" r:id="rId93"/>
+    <hyperlink ref="D97" r:id="rId94"/>
+    <hyperlink ref="D87" r:id="rId95"/>
+    <hyperlink ref="D80" r:id="rId96"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId97"/>

</xml_diff>

<commit_message>
typo fixed in database
</commit_message>
<xml_diff>
--- a/data/Updated_Table_Mislan_2020_v2.xlsx
+++ b/data/Updated_Table_Mislan_2020_v2.xlsx
@@ -1262,7 +1262,7 @@
   <dimension ref="A1:G98"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A61" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E81" sqref="E81"/>
+      <selection activeCell="F76" sqref="F76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2946,7 +2946,7 @@
         <v>6</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G79" s="1" t="s">
         <v>264</v>

</xml_diff>